<commit_message>
Updates made to vax efficacy random values assigned to single dose.
</commit_message>
<xml_diff>
--- a/Params/VaxEfficacyRandVal.xlsx
+++ b/Params/VaxEfficacyRandVal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clh89/MATLAB/Projects/KenyaModel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clh89/MATLAB/Projects/Kenya_treatment/Params/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A777A323-DFAA-9E4B-81C6-981036ADA72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE52CE7-520C-324A-8A42-2BA36383B8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23140" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VaxEfficacyRandVal" sheetId="1" r:id="rId1"/>
@@ -351,311 +351,311 @@
   <dimension ref="A1:CV1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:100" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>0.98944765963765402</v>
+        <v>0.98302901785187102</v>
       </c>
       <c r="B1">
-        <v>0.98235682872175301</v>
+        <v>0.97569909610059602</v>
       </c>
       <c r="C1">
-        <v>0.97220567243321099</v>
+        <v>0.96661691542948802</v>
       </c>
       <c r="D1">
-        <v>0.96964314323129097</v>
+        <v>0.96449336079088199</v>
       </c>
       <c r="E1">
-        <v>0.95004762895293704</v>
+        <v>0.94966027691702903</v>
       </c>
       <c r="F1">
-        <v>0.99139012179031705</v>
+        <v>0.992714189094005</v>
       </c>
       <c r="G1">
-        <v>0.95437531342958604</v>
+        <v>0.98527778542775402</v>
       </c>
       <c r="H1">
-        <v>0.97047853645363102</v>
+        <v>0.98073908405315802</v>
       </c>
       <c r="I1">
-        <v>0.98936953005058703</v>
+        <v>0.95276479738130904</v>
       </c>
       <c r="J1">
-        <v>0.99926993826383803</v>
+        <v>0.96517960579049</v>
       </c>
       <c r="K1">
-        <v>0.92804737251648795</v>
+        <v>0.98294133220660895</v>
       </c>
       <c r="L1">
-        <v>0.98787816687938401</v>
+        <v>0.94764711149346204</v>
       </c>
       <c r="M1">
-        <v>0.99548864389633596</v>
+        <v>0.99738600015754397</v>
       </c>
       <c r="N1">
-        <v>0.98202521058447501</v>
+        <v>0.93488189171523906</v>
       </c>
       <c r="O1">
-        <v>0.99514313898703499</v>
+        <v>0.98130292320127099</v>
       </c>
       <c r="P1">
-        <v>0.99196198147641201</v>
+        <v>0.99063105173537902</v>
       </c>
       <c r="Q1">
-        <v>0.99048391174260797</v>
+        <v>0.97538098617963898</v>
       </c>
       <c r="R1">
-        <v>0.99864044851476896</v>
+        <v>0.99013459154161498</v>
       </c>
       <c r="S1">
-        <v>0.91129143463773499</v>
+        <v>0.98596822114529803</v>
       </c>
       <c r="T1">
-        <v>0.96852674115016402</v>
+        <v>0.984211409284106</v>
       </c>
       <c r="U1">
-        <v>0.99602226404856997</v>
+        <v>0.99595648393467695</v>
       </c>
       <c r="V1">
-        <v>0.95257570395785096</v>
+        <v>0.92443543793937799</v>
       </c>
       <c r="W1">
-        <v>0.98402603343779405</v>
+        <v>0.96358490499643801</v>
       </c>
       <c r="X1">
-        <v>0.942506592420158</v>
+        <v>0.991421136988483</v>
       </c>
       <c r="Y1">
-        <v>0.97722635481392905</v>
+        <v>0.95146410767954204</v>
       </c>
       <c r="Z1">
-        <v>0.98429127517505699</v>
+        <v>0.97732868521638905</v>
       </c>
       <c r="AA1">
-        <v>0.98599913877856304</v>
+        <v>0.91950310395177803</v>
       </c>
       <c r="AB1">
-        <v>0.99149961074237303</v>
+        <v>0.92576811046260399</v>
       </c>
       <c r="AC1">
-        <v>0.98174747456585998</v>
+        <v>0.93577149011205196</v>
       </c>
       <c r="AD1">
-        <v>0.99685211997401402</v>
+        <v>0.94442478115643802</v>
       </c>
       <c r="AE1">
-        <v>0.99591298636802905</v>
+        <v>0.97095597095934105</v>
       </c>
       <c r="AF1">
-        <v>0.98647833728669398</v>
+        <v>0.97759225803972905</v>
       </c>
       <c r="AG1">
-        <v>0.98776080841115499</v>
+        <v>0.97932299820070501</v>
       </c>
       <c r="AH1">
-        <v>0.91884008023196695</v>
+        <v>0.98540887483963302</v>
       </c>
       <c r="AI1">
-        <v>0.97795222838935503</v>
+        <v>0.97511592048051998</v>
       </c>
       <c r="AJ1">
-        <v>0.96343886516273602</v>
+        <v>0.99271738719040603</v>
       </c>
       <c r="AK1">
-        <v>0.97605159765998295</v>
+        <v>0.88542299210890696</v>
       </c>
       <c r="AL1">
-        <v>0.97656293952851903</v>
+        <v>0.99125685264181795</v>
       </c>
       <c r="AM1">
-        <v>0.98223774713765599</v>
+        <v>0.97981986307005098</v>
       </c>
       <c r="AN1">
-        <v>0.93976689212648501</v>
+        <v>0.98117666706284601</v>
       </c>
       <c r="AO1">
-        <v>0.96988950868735602</v>
+        <v>0.929072850608333</v>
       </c>
       <c r="AP1">
-        <v>0.96543156851205503</v>
+        <v>0.971605876422038</v>
       </c>
       <c r="AQ1">
-        <v>0.95580300670745699</v>
+        <v>0.95955799089417204</v>
       </c>
       <c r="AR1">
-        <v>0.98842884912844997</v>
+        <v>0.96991711011649095</v>
       </c>
       <c r="AS1">
-        <v>0.99507944916072599</v>
+        <v>0.97036738475080297</v>
       </c>
       <c r="AT1">
-        <v>0.99552030153353099</v>
+        <v>0.97558465983076004</v>
       </c>
       <c r="AU1">
-        <v>0.96057838478593804</v>
+        <v>0.94257075293368897</v>
       </c>
       <c r="AV1">
-        <v>0.95099575756041799</v>
+        <v>0.96469515473795597</v>
       </c>
       <c r="AW1">
-        <v>0.97292668843989005</v>
+        <v>0.96111428112824204</v>
       </c>
       <c r="AX1">
-        <v>0.98822101774746196</v>
+        <v>0.95380710297596405</v>
       </c>
       <c r="AY1">
-        <v>0.99968493567485395</v>
+        <v>0.98190038150445702</v>
       </c>
       <c r="AZ1">
-        <v>0.99169843594993701</v>
+        <v>0.99004425828125098</v>
       </c>
       <c r="BA1">
-        <v>0.99140631135917801</v>
+        <v>0.99067710564327405</v>
       </c>
       <c r="BB1">
-        <v>0.98377139248859502</v>
+        <v>0.95736639110752497</v>
       </c>
       <c r="BC1">
-        <v>0.99657940882754703</v>
+        <v>0.950333690683559</v>
       </c>
       <c r="BD1">
-        <v>0.96718084678701299</v>
+        <v>0.96722472063138298</v>
       </c>
       <c r="BE1">
-        <v>0.97972877460409902</v>
+        <v>0.98167390663607001</v>
       </c>
       <c r="BF1">
-        <v>0.97478227247365301</v>
+        <v>0.99855105206241201</v>
       </c>
       <c r="BG1">
-        <v>0.95542642992606297</v>
+        <v>0.90894520982402005</v>
       </c>
       <c r="BH1">
-        <v>0.98578451126052102</v>
+        <v>0.98564824152854802</v>
       </c>
       <c r="BI1">
-        <v>0.93403771705887795</v>
+        <v>0.98529713699147903</v>
       </c>
       <c r="BJ1">
-        <v>0.98209394341799805</v>
+        <v>0.97707688557274197</v>
       </c>
       <c r="BK1">
-        <v>0.95887017785286499</v>
+        <v>0.99228114739644901</v>
       </c>
       <c r="BL1">
-        <v>0.95194871694789696</v>
+        <v>0.96250221069644704</v>
       </c>
       <c r="BM1">
-        <v>0.98476698507232596</v>
+        <v>0.97322424858703105</v>
       </c>
       <c r="BN1">
-        <v>0.94298547788878595</v>
+        <v>0.96881156591151896</v>
       </c>
       <c r="BO1">
-        <v>0.96422993170483295</v>
+        <v>0.95353125645708703</v>
       </c>
       <c r="BP1">
-        <v>0.99052774107087305</v>
+        <v>0.97910212946813302</v>
       </c>
       <c r="BQ1">
-        <v>0.99009747187772601</v>
+        <v>0.93876611578412095</v>
       </c>
       <c r="BR1">
-        <v>0.98250501725763495</v>
+        <v>0.97544677312374894</v>
       </c>
       <c r="BS1">
-        <v>0.99514668832721898</v>
+        <v>0.95607964595454098</v>
       </c>
       <c r="BT1">
-        <v>0.96324285384657604</v>
+        <v>0.95101425511876103</v>
       </c>
       <c r="BU1">
-        <v>0.98279646503026596</v>
+        <v>0.97806836671944897</v>
       </c>
       <c r="BV1">
-        <v>0.98526673564091405</v>
+        <v>0.91018555309710103</v>
       </c>
       <c r="BW1">
-        <v>0.99447230070907799</v>
+        <v>0.94475132778253401</v>
       </c>
       <c r="BX1">
-        <v>0.97663902926808899</v>
+        <v>0.96017277083785402</v>
       </c>
       <c r="BY1">
-        <v>0.99267194922681201</v>
+        <v>0.98426225576308402</v>
       </c>
       <c r="BZ1">
-        <v>0.99858536877071002</v>
+        <v>0.98376612032337096</v>
       </c>
       <c r="CA1">
-        <v>0.98599382681922798</v>
+        <v>0.97584182913752804</v>
       </c>
       <c r="CB1">
-        <v>0.99842893159383395</v>
+        <v>0.99013963618517298</v>
       </c>
       <c r="CC1">
-        <v>0.97700716755430095</v>
+        <v>0.95940626150571495</v>
       </c>
       <c r="CD1">
-        <v>0.96071867246073495</v>
+        <v>0.97612361454225505</v>
       </c>
       <c r="CE1">
-        <v>0.97069942225144501</v>
+        <v>0.97857339647901398</v>
       </c>
       <c r="CF1">
-        <v>0.99072125074334505</v>
+        <v>0.98920005060975102</v>
       </c>
       <c r="CG1">
-        <v>0.99342438713914905</v>
+        <v>0.97043463694231502</v>
       </c>
       <c r="CH1">
-        <v>0.99512712611528098</v>
+        <v>0.98684651508293297</v>
       </c>
       <c r="CI1">
-        <v>0.97016854984998402</v>
+        <v>0.99584228821217502</v>
       </c>
       <c r="CJ1">
-        <v>0.99443269631284603</v>
+        <v>0.97931751948377199</v>
       </c>
       <c r="CK1">
-        <v>0.98821222555967403</v>
+        <v>0.94111563409874399</v>
       </c>
       <c r="CL1">
-        <v>0.98304209800461695</v>
+        <v>0.99552497984493904</v>
       </c>
       <c r="CM1">
-        <v>0.99088833066612103</v>
+        <v>0.970760946882406</v>
       </c>
       <c r="CN1">
-        <v>0.96440890261604095</v>
+        <v>0.95747277435417699</v>
       </c>
       <c r="CO1">
-        <v>0.97189299476699997</v>
+        <v>0.965362009635921</v>
       </c>
       <c r="CP1">
-        <v>0.99456910913455299</v>
+        <v>0.98448760502085997</v>
       </c>
       <c r="CQ1">
-        <v>0.97754701321637205</v>
+        <v>0.98780602538000095</v>
       </c>
       <c r="CR1">
-        <v>0.97340119794695301</v>
+        <v>0.99011184644424699</v>
       </c>
       <c r="CS1">
-        <v>0.98688524260300903</v>
+        <v>0.96492430236343396</v>
       </c>
       <c r="CT1">
-        <v>0.99940463220952502</v>
+        <v>0.98914598646981999</v>
       </c>
       <c r="CU1">
-        <v>0.860132585030004</v>
+        <v>0.98166435253159601</v>
       </c>
       <c r="CV1">
-        <v>0.99783837041013701</v>
+        <v>0.97636222212081503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>